<commit_message>
Minor fixes and removed namespace std
</commit_message>
<xml_diff>
--- a/BaseballProject/Souvenirs.xlsx
+++ b/BaseballProject/Souvenirs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="35">
   <si>
     <t>Chase Field</t>
   </si>
@@ -28,16 +28,16 @@
     <t>Team pennant</t>
   </si>
   <si>
+    <t>SunTrust Park</t>
+  </si>
+  <si>
     <t>Autographed baseball</t>
   </si>
   <si>
+    <t>Oriole Park at Camden Yards</t>
+  </si>
+  <si>
     <t>Team jersey</t>
-  </si>
-  <si>
-    <t>SunTrust Park</t>
-  </si>
-  <si>
-    <t>Oriole Park at Camden Yards</t>
   </si>
   <si>
     <t>Fenway Park</t>
@@ -446,7 +446,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:C150"/>
+  <dimension ref="A2:C148"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
@@ -487,46 +487,46 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>25.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>199.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C7">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C8">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="9">
@@ -534,10 +534,10 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>17.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="10">
@@ -545,65 +545,65 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10">
-        <v>25.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C11">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C12">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C13">
-        <v>17.99</v>
+        <v>199.99</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>25.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C15">
-        <v>199.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="16">
@@ -611,10 +611,10 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C16">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -622,10 +622,10 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C17">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -633,32 +633,32 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C18">
-        <v>17.99</v>
+        <v>199.99</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <v>25.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C20">
-        <v>199.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -666,10 +666,10 @@
         <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C21">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -677,10 +677,10 @@
         <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C22">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -688,32 +688,32 @@
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C23">
-        <v>17.99</v>
+        <v>199.99</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C24">
-        <v>25.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C25">
-        <v>199.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -721,10 +721,10 @@
         <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C26">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -732,10 +732,10 @@
         <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C27">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -743,32 +743,32 @@
         <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C28">
-        <v>17.99</v>
+        <v>199.99</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C29">
-        <v>25.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C30">
-        <v>199.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -776,10 +776,10 @@
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C31">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -787,10 +787,10 @@
         <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C32">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -798,32 +798,32 @@
         <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C33">
-        <v>17.99</v>
+        <v>199.99</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B34" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C34">
-        <v>25.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B35" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C35">
-        <v>199.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -831,10 +831,10 @@
         <v>12</v>
       </c>
       <c r="B36" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C36">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -842,10 +842,10 @@
         <v>12</v>
       </c>
       <c r="B37" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C37">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -853,32 +853,32 @@
         <v>12</v>
       </c>
       <c r="B38" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C38">
-        <v>17.99</v>
+        <v>199.99</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B39" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C39">
-        <v>25.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B40" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C40">
-        <v>199.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -886,10 +886,10 @@
         <v>13</v>
       </c>
       <c r="B41" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C41">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -897,10 +897,10 @@
         <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C42">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -908,32 +908,32 @@
         <v>13</v>
       </c>
       <c r="B43" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C43">
-        <v>17.99</v>
+        <v>199.99</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C44">
-        <v>25.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B45" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C45">
-        <v>199.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -941,10 +941,10 @@
         <v>14</v>
       </c>
       <c r="B46" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C46">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -952,10 +952,10 @@
         <v>14</v>
       </c>
       <c r="B47" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C47">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -963,32 +963,32 @@
         <v>14</v>
       </c>
       <c r="B48" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C48">
-        <v>17.99</v>
+        <v>199.99</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B49" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C49">
-        <v>25.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B50" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C50">
-        <v>199.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -996,10 +996,10 @@
         <v>15</v>
       </c>
       <c r="B51" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C51">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1007,10 +1007,10 @@
         <v>15</v>
       </c>
       <c r="B52" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C52">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1018,32 +1018,32 @@
         <v>15</v>
       </c>
       <c r="B53" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C53">
-        <v>17.99</v>
+        <v>199.99</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B54" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C54">
-        <v>25.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B55" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C55">
-        <v>199.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1051,10 +1051,10 @@
         <v>16</v>
       </c>
       <c r="B56" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C56">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1062,10 +1062,10 @@
         <v>16</v>
       </c>
       <c r="B57" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C57">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1073,32 +1073,32 @@
         <v>16</v>
       </c>
       <c r="B58" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C58">
-        <v>17.99</v>
+        <v>199.99</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B59" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C59">
-        <v>25.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B60" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C60">
-        <v>199.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1106,10 +1106,10 @@
         <v>17</v>
       </c>
       <c r="B61" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C61">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1117,10 +1117,10 @@
         <v>17</v>
       </c>
       <c r="B62" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C62">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1128,32 +1128,32 @@
         <v>17</v>
       </c>
       <c r="B63" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C63">
-        <v>17.99</v>
+        <v>199.99</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B64" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C64">
-        <v>25.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B65" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C65">
-        <v>199.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1161,10 +1161,10 @@
         <v>18</v>
       </c>
       <c r="B66" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C66">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1172,10 +1172,10 @@
         <v>18</v>
       </c>
       <c r="B67" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C67">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1183,32 +1183,32 @@
         <v>18</v>
       </c>
       <c r="B68" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C68">
-        <v>17.99</v>
+        <v>199.99</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B69" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C69">
-        <v>25.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B70" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C70">
-        <v>199.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1216,10 +1216,10 @@
         <v>19</v>
       </c>
       <c r="B71" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C71">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1227,10 +1227,10 @@
         <v>19</v>
       </c>
       <c r="B72" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C72">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1238,32 +1238,32 @@
         <v>19</v>
       </c>
       <c r="B73" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C73">
-        <v>17.99</v>
+        <v>199.99</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B74" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C74">
-        <v>25.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B75" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C75">
-        <v>199.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1271,10 +1271,10 @@
         <v>20</v>
       </c>
       <c r="B76" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C76">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1282,10 +1282,10 @@
         <v>20</v>
       </c>
       <c r="B77" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C77">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1293,32 +1293,32 @@
         <v>20</v>
       </c>
       <c r="B78" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C78">
-        <v>17.99</v>
+        <v>199.99</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B79" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C79">
-        <v>25.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B80" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C80">
-        <v>199.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1326,10 +1326,10 @@
         <v>21</v>
       </c>
       <c r="B81" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C81">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1337,10 +1337,10 @@
         <v>21</v>
       </c>
       <c r="B82" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C82">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1348,32 +1348,32 @@
         <v>21</v>
       </c>
       <c r="B83" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C83">
-        <v>17.99</v>
+        <v>199.99</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B84" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C84">
-        <v>25.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B85" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C85">
-        <v>199.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1381,10 +1381,10 @@
         <v>22</v>
       </c>
       <c r="B86" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C86">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1392,10 +1392,10 @@
         <v>22</v>
       </c>
       <c r="B87" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C87">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1403,32 +1403,32 @@
         <v>22</v>
       </c>
       <c r="B88" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C88">
-        <v>17.99</v>
+        <v>199.99</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B89" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C89">
-        <v>25.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B90" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C90">
-        <v>199.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1436,10 +1436,10 @@
         <v>23</v>
       </c>
       <c r="B91" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C91">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -1447,10 +1447,10 @@
         <v>23</v>
       </c>
       <c r="B92" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C92">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -1458,32 +1458,32 @@
         <v>23</v>
       </c>
       <c r="B93" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C93">
-        <v>17.99</v>
+        <v>199.99</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B94" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C94">
-        <v>25.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B95" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C95">
-        <v>199.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1491,10 +1491,10 @@
         <v>24</v>
       </c>
       <c r="B96" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C96">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1502,10 +1502,10 @@
         <v>24</v>
       </c>
       <c r="B97" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C97">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1513,32 +1513,32 @@
         <v>24</v>
       </c>
       <c r="B98" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C98">
-        <v>17.99</v>
+        <v>199.99</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B99" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C99">
-        <v>25.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B100" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C100">
-        <v>199.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -1546,10 +1546,10 @@
         <v>25</v>
       </c>
       <c r="B101" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C101">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -1557,10 +1557,10 @@
         <v>25</v>
       </c>
       <c r="B102" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C102">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -1568,32 +1568,32 @@
         <v>25</v>
       </c>
       <c r="B103" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C103">
-        <v>17.99</v>
+        <v>199.99</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B104" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C104">
-        <v>25.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B105" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C105">
-        <v>199.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -1601,10 +1601,10 @@
         <v>26</v>
       </c>
       <c r="B106" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C106">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -1612,10 +1612,10 @@
         <v>26</v>
       </c>
       <c r="B107" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C107">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -1623,32 +1623,32 @@
         <v>26</v>
       </c>
       <c r="B108" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C108">
-        <v>17.99</v>
+        <v>199.99</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B109" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C109">
-        <v>25.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B110" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C110">
-        <v>199.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -1656,10 +1656,10 @@
         <v>27</v>
       </c>
       <c r="B111" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C111">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -1667,10 +1667,10 @@
         <v>27</v>
       </c>
       <c r="B112" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C112">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -1678,32 +1678,32 @@
         <v>27</v>
       </c>
       <c r="B113" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C113">
-        <v>17.99</v>
+        <v>199.99</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B114" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C114">
-        <v>25.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B115" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C115">
-        <v>199.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -1711,10 +1711,10 @@
         <v>28</v>
       </c>
       <c r="B116" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C116">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -1722,10 +1722,10 @@
         <v>28</v>
       </c>
       <c r="B117" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C117">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -1733,32 +1733,32 @@
         <v>28</v>
       </c>
       <c r="B118" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C118">
-        <v>17.99</v>
+        <v>199.99</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B119" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C119">
-        <v>25.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B120" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C120">
-        <v>199.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -1766,10 +1766,10 @@
         <v>29</v>
       </c>
       <c r="B121" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C121">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -1777,10 +1777,10 @@
         <v>29</v>
       </c>
       <c r="B122" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C122">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -1788,32 +1788,32 @@
         <v>29</v>
       </c>
       <c r="B123" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C123">
-        <v>17.99</v>
+        <v>199.99</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B124" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C124">
-        <v>25.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B125" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C125">
-        <v>199.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -1821,10 +1821,10 @@
         <v>30</v>
       </c>
       <c r="B126" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C126">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -1832,10 +1832,10 @@
         <v>30</v>
       </c>
       <c r="B127" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C127">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -1843,32 +1843,32 @@
         <v>30</v>
       </c>
       <c r="B128" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C128">
-        <v>17.99</v>
+        <v>199.99</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B129" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C129">
-        <v>25.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B130" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C130">
-        <v>199.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -1876,10 +1876,10 @@
         <v>31</v>
       </c>
       <c r="B131" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C131">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -1887,10 +1887,10 @@
         <v>31</v>
       </c>
       <c r="B132" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C132">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -1898,32 +1898,32 @@
         <v>31</v>
       </c>
       <c r="B133" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C133">
-        <v>17.99</v>
+        <v>199.99</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B134" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C134">
-        <v>25.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B135" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C135">
-        <v>199.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -1931,10 +1931,10 @@
         <v>32</v>
       </c>
       <c r="B136" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C136">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -1942,10 +1942,10 @@
         <v>32</v>
       </c>
       <c r="B137" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C137">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -1953,32 +1953,32 @@
         <v>32</v>
       </c>
       <c r="B138" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C138">
-        <v>17.99</v>
+        <v>199.99</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B139" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C139">
-        <v>25.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B140" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C140">
-        <v>199.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -1986,10 +1986,10 @@
         <v>33</v>
       </c>
       <c r="B141" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C141">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -1997,10 +1997,10 @@
         <v>33</v>
       </c>
       <c r="B142" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C142">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -2008,32 +2008,32 @@
         <v>33</v>
       </c>
       <c r="B143" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C143">
-        <v>17.99</v>
+        <v>199.99</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B144" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C144">
-        <v>25.99</v>
+        <v>22.99</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B145" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C145">
-        <v>199.99</v>
+        <v>89.39</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -2041,10 +2041,10 @@
         <v>34</v>
       </c>
       <c r="B146" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C146">
-        <v>22.99</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -2052,10 +2052,10 @@
         <v>34</v>
       </c>
       <c r="B147" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C147">
-        <v>89.39</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -2063,31 +2063,9 @@
         <v>34</v>
       </c>
       <c r="B148" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C148">
-        <v>17.99</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3">
-      <c r="A149" t="s">
-        <v>34</v>
-      </c>
-      <c r="B149" t="s">
-        <v>4</v>
-      </c>
-      <c r="C149">
-        <v>25.99</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3">
-      <c r="A150" t="s">
-        <v>34</v>
-      </c>
-      <c r="B150" t="s">
-        <v>5</v>
-      </c>
-      <c r="C150">
         <v>199.99</v>
       </c>
     </row>

</xml_diff>